<commit_message>
fixed test numbering in manual cases after review
</commit_message>
<xml_diff>
--- a/ManualTests/DemoBlazeMasterTestSuite.xlsx
+++ b/ManualTests/DemoBlazeMasterTestSuite.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AZT251477\Downloads\Sertis\Automation\ManualTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KaranGit\Automation\ManualTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3237943F-0C9E-41E2-B31E-2439D282CFCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A641AB0B-C9AB-4102-B309-C5DF60DA20F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Test cases" sheetId="1" r:id="rId1"/>
@@ -975,21 +975,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.90625" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" customWidth="1"/>
-    <col min="4" max="4" width="24.54296875" customWidth="1"/>
-    <col min="5" max="5" width="35.453125" customWidth="1"/>
-    <col min="6" max="6" width="43.81640625" customWidth="1"/>
+    <col min="1" max="1" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" customWidth="1"/>
+    <col min="5" max="5" width="35.44140625" customWidth="1"/>
+    <col min="6" max="6" width="43.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="348" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="116" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" s="1" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" s="1" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" s="1" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1305,9 +1305,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="1" customFormat="1" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" s="1" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>49</v>
@@ -1334,21 +1334,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A100D6FF-26DD-4E00-8E46-37F1BE79894F}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.90625" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" customWidth="1"/>
-    <col min="5" max="5" width="35.453125" customWidth="1"/>
-    <col min="6" max="6" width="43.81640625" customWidth="1"/>
+    <col min="1" max="1" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="35.44140625" customWidth="1"/>
+    <col min="6" max="6" width="43.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="145" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" s="1" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" s="1" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" ht="290" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" s="1" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="174" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="261" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="261" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" s="1" customFormat="1" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" s="1" customFormat="1" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="290" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" s="1" customFormat="1" ht="288" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" s="1" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" s="1" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" s="1" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" s="1" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1648,13 +1648,13 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="E18" s="2"/>

</xml_diff>